<commit_message>
Revert "Revert "Week 4""
This reverts commit eafdb2c45f11f40ca420437e5120bf2f205612c9.
</commit_message>
<xml_diff>
--- a/EM-Week-3.xlsx
+++ b/EM-Week-3.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Week 3" sheetId="1" r:id="rId1"/>
+    <sheet name="Week 4" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -668,55 +668,55 @@
         <v>23</v>
       </c>
       <c r="D3">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E3">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G3">
-        <v>56.52</v>
+        <v>55.56</v>
       </c>
       <c r="H3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I3">
-        <v>8074</v>
+        <v>9810</v>
       </c>
       <c r="J3">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="K3">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="L3">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="M3">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="N3">
-        <v>30</v>
+        <v>28.57</v>
       </c>
       <c r="O3">
-        <v>351</v>
+        <v>363.3</v>
       </c>
       <c r="P3">
-        <v>0.78</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="Q3">
         <v>0.7</v>
       </c>
       <c r="R3">
-        <v>1.43</v>
+        <v>1.44</v>
       </c>
       <c r="S3">
-        <v>2.61</v>
+        <v>2.85</v>
       </c>
       <c r="T3">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="U3">
         <v>1</v>
@@ -736,58 +736,58 @@
         <v>23</v>
       </c>
       <c r="D4">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E4">
+        <v>15</v>
+      </c>
+      <c r="F4">
         <v>13</v>
       </c>
-      <c r="F4">
-        <v>11</v>
-      </c>
       <c r="G4">
-        <v>54.17</v>
+        <v>53.57</v>
       </c>
       <c r="H4">
         <v>7</v>
       </c>
       <c r="I4">
-        <v>9072</v>
+        <v>10777</v>
       </c>
       <c r="J4">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="K4">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="L4">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="M4">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="N4">
-        <v>35.38</v>
+        <v>35.8</v>
       </c>
       <c r="O4">
-        <v>378</v>
+        <v>384.9</v>
       </c>
       <c r="P4">
-        <v>0.96</v>
+        <v>1.04</v>
       </c>
       <c r="Q4">
         <v>0.54</v>
       </c>
       <c r="R4">
-        <v>1.46</v>
+        <v>1.29</v>
       </c>
       <c r="S4">
-        <v>2.71</v>
+        <v>2.89</v>
       </c>
       <c r="T4">
         <v>2</v>
       </c>
       <c r="U4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V4">
         <v>1</v>
@@ -872,55 +872,55 @@
         <v>23</v>
       </c>
       <c r="D6">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E6">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F6">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G6">
-        <v>61.11</v>
+        <v>59.09</v>
       </c>
       <c r="H6">
         <v>3</v>
       </c>
       <c r="I6">
-        <v>6956</v>
+        <v>8438</v>
       </c>
       <c r="J6">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K6">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L6">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="M6">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="N6">
-        <v>31.91</v>
+        <v>29.31</v>
       </c>
       <c r="O6">
-        <v>386.4</v>
+        <v>383.5</v>
       </c>
       <c r="P6">
-        <v>0.83</v>
+        <v>0.77</v>
       </c>
       <c r="Q6">
-        <v>1.06</v>
+        <v>1</v>
       </c>
       <c r="R6">
-        <v>1.17</v>
+        <v>1.09</v>
       </c>
       <c r="S6">
-        <v>2.61</v>
+        <v>2.64</v>
       </c>
       <c r="T6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="U6">
         <v>1</v>
@@ -1008,61 +1008,61 @@
         <v>28</v>
       </c>
       <c r="D8">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="E8">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F8">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G8">
-        <v>41.67</v>
+        <v>46.88</v>
       </c>
       <c r="H8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I8">
-        <v>8397</v>
+        <v>11341</v>
       </c>
       <c r="J8">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="K8">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="L8">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="M8">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="N8">
-        <v>18.42</v>
+        <v>22</v>
       </c>
       <c r="O8">
-        <v>349.9</v>
+        <v>354.4</v>
       </c>
       <c r="P8">
-        <v>0.58</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="Q8">
-        <v>0.54</v>
+        <v>0.72</v>
       </c>
       <c r="R8">
-        <v>1.46</v>
+        <v>1.25</v>
       </c>
       <c r="S8">
-        <v>3.17</v>
+        <v>3.13</v>
       </c>
       <c r="T8">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="U8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W8">
         <v>4</v>
@@ -1076,64 +1076,64 @@
         <v>28</v>
       </c>
       <c r="D9">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E9">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F9">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G9">
-        <v>43.48</v>
+        <v>48.39</v>
       </c>
       <c r="H9">
+        <v>6</v>
+      </c>
+      <c r="I9">
+        <v>12707</v>
+      </c>
+      <c r="J9">
+        <v>31</v>
+      </c>
+      <c r="K9">
+        <v>12</v>
+      </c>
+      <c r="L9">
+        <v>53</v>
+      </c>
+      <c r="M9">
+        <v>80</v>
+      </c>
+      <c r="N9">
+        <v>38.75</v>
+      </c>
+      <c r="O9">
+        <v>409.9</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>0.39</v>
+      </c>
+      <c r="R9">
+        <v>1.71</v>
+      </c>
+      <c r="S9">
+        <v>2.58</v>
+      </c>
+      <c r="T9">
+        <v>3</v>
+      </c>
+      <c r="U9">
         <v>4</v>
       </c>
-      <c r="I9">
-        <v>8947</v>
-      </c>
-      <c r="J9">
-        <v>18</v>
-      </c>
-      <c r="K9">
-        <v>10</v>
-      </c>
-      <c r="L9">
-        <v>39</v>
-      </c>
-      <c r="M9">
-        <v>60</v>
-      </c>
-      <c r="N9">
-        <v>30</v>
-      </c>
-      <c r="O9">
-        <v>389</v>
-      </c>
-      <c r="P9">
-        <v>0.78</v>
-      </c>
-      <c r="Q9">
-        <v>0.43</v>
-      </c>
-      <c r="R9">
-        <v>1.7</v>
-      </c>
-      <c r="S9">
-        <v>2.61</v>
-      </c>
-      <c r="T9">
-        <v>2</v>
-      </c>
-      <c r="U9">
-        <v>2</v>
-      </c>
       <c r="V9">
         <v>0</v>
       </c>
       <c r="W9">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="2:23">
@@ -1144,58 +1144,58 @@
         <v>28</v>
       </c>
       <c r="D10">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E10">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F10">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G10">
-        <v>50</v>
+        <v>56.25</v>
       </c>
       <c r="H10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I10">
-        <v>2715</v>
+        <v>5866</v>
       </c>
       <c r="J10">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="K10">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="L10">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="M10">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="N10">
-        <v>25</v>
+        <v>37.5</v>
       </c>
       <c r="O10">
-        <v>339.4</v>
+        <v>366.6</v>
       </c>
       <c r="P10">
-        <v>0.75</v>
+        <v>1.13</v>
       </c>
       <c r="Q10">
-        <v>0.25</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="R10">
-        <v>1.88</v>
+        <v>1.31</v>
       </c>
       <c r="S10">
         <v>3</v>
       </c>
       <c r="T10">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="U10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V10">
         <v>0</v>
@@ -1212,64 +1212,64 @@
         <v>33</v>
       </c>
       <c r="D11">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E11">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F11">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G11">
-        <v>52.17</v>
+        <v>48.39</v>
       </c>
       <c r="H11">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I11">
-        <v>9272</v>
+        <v>12375</v>
       </c>
       <c r="J11">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="K11">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="L11">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="M11">
-        <v>69</v>
+        <v>91</v>
       </c>
       <c r="N11">
-        <v>31.88</v>
+        <v>29.67</v>
       </c>
       <c r="O11">
-        <v>403.1</v>
+        <v>399.2</v>
       </c>
       <c r="P11">
-        <v>0.96</v>
+        <v>0.87</v>
       </c>
       <c r="Q11">
-        <v>0.78</v>
+        <v>0.77</v>
       </c>
       <c r="R11">
-        <v>1.78</v>
+        <v>1.87</v>
       </c>
       <c r="S11">
+        <v>2.94</v>
+      </c>
+      <c r="T11">
+        <v>7</v>
+      </c>
+      <c r="U11">
+        <v>2</v>
+      </c>
+      <c r="V11">
         <v>3</v>
       </c>
-      <c r="T11">
-        <v>5</v>
-      </c>
-      <c r="U11">
-        <v>1</v>
-      </c>
-      <c r="V11">
-        <v>2</v>
-      </c>
       <c r="W11">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="2:23">
@@ -1280,52 +1280,52 @@
         <v>33</v>
       </c>
       <c r="D12">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E12">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F12">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G12">
-        <v>57.14</v>
+        <v>50</v>
       </c>
       <c r="H12">
         <v>3</v>
       </c>
       <c r="I12">
-        <v>7431</v>
+        <v>8722</v>
       </c>
       <c r="J12">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="K12">
         <v>13</v>
       </c>
       <c r="L12">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="M12">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="N12">
-        <v>31.91</v>
+        <v>33.33</v>
       </c>
       <c r="O12">
-        <v>353.9</v>
+        <v>335.5</v>
       </c>
       <c r="P12">
-        <v>0.71</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="Q12">
-        <v>0.62</v>
+        <v>0.5</v>
       </c>
       <c r="R12">
-        <v>1.29</v>
+        <v>1.31</v>
       </c>
       <c r="S12">
-        <v>2.24</v>
+        <v>2.08</v>
       </c>
       <c r="T12">
         <v>3</v>
@@ -1348,52 +1348,52 @@
         <v>33</v>
       </c>
       <c r="D13">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E13">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F13">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G13">
-        <v>35.71</v>
+        <v>35</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
-        <v>3556</v>
+        <v>4839</v>
       </c>
       <c r="J13">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K13">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="L13">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="M13">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="N13">
-        <v>18.52</v>
+        <v>16.67</v>
       </c>
       <c r="O13">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="P13">
-        <v>0.36</v>
+        <v>0.3</v>
       </c>
       <c r="Q13">
-        <v>0.36</v>
+        <v>0.4</v>
       </c>
       <c r="R13">
-        <v>0.93</v>
+        <v>0.9</v>
       </c>
       <c r="S13">
-        <v>1.93</v>
+        <v>1.8</v>
       </c>
       <c r="T13">
         <v>2</v>
@@ -1416,64 +1416,64 @@
         <v>33</v>
       </c>
       <c r="D14">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E14">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F14">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G14">
-        <v>50</v>
+        <v>52.63</v>
       </c>
       <c r="H14">
+        <v>6</v>
+      </c>
+      <c r="I14">
+        <v>7510</v>
+      </c>
+      <c r="J14">
+        <v>25</v>
+      </c>
+      <c r="K14">
+        <v>13</v>
+      </c>
+      <c r="L14">
+        <v>16</v>
+      </c>
+      <c r="M14">
+        <v>60</v>
+      </c>
+      <c r="N14">
+        <v>41.67</v>
+      </c>
+      <c r="O14">
+        <v>395.3</v>
+      </c>
+      <c r="P14">
+        <v>1.32</v>
+      </c>
+      <c r="Q14">
+        <v>0.68</v>
+      </c>
+      <c r="R14">
+        <v>0.84</v>
+      </c>
+      <c r="S14">
+        <v>3.16</v>
+      </c>
+      <c r="T14">
+        <v>3</v>
+      </c>
+      <c r="U14">
         <v>4</v>
       </c>
-      <c r="I14">
-        <v>5514</v>
-      </c>
-      <c r="J14">
-        <v>19</v>
-      </c>
-      <c r="K14">
-        <v>10</v>
-      </c>
-      <c r="L14">
-        <v>9</v>
-      </c>
-      <c r="M14">
-        <v>46</v>
-      </c>
-      <c r="N14">
-        <v>41.3</v>
-      </c>
-      <c r="O14">
-        <v>393.9</v>
-      </c>
-      <c r="P14">
-        <v>1.36</v>
-      </c>
-      <c r="Q14">
-        <v>0.71</v>
-      </c>
-      <c r="R14">
-        <v>0.64</v>
-      </c>
-      <c r="S14">
-        <v>3.29</v>
-      </c>
-      <c r="T14">
-        <v>2</v>
-      </c>
-      <c r="U14">
-        <v>3</v>
-      </c>
       <c r="V14">
         <v>1</v>
       </c>
       <c r="W14">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="2:23">
@@ -1484,55 +1484,55 @@
         <v>38</v>
       </c>
       <c r="D15">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E15">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F15">
         <v>15</v>
       </c>
       <c r="G15">
-        <v>31.82</v>
+        <v>42.31</v>
       </c>
       <c r="H15">
         <v>4</v>
       </c>
       <c r="I15">
-        <v>6986</v>
+        <v>8156</v>
       </c>
       <c r="J15">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="K15">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="L15">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="M15">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="N15">
-        <v>27.08</v>
+        <v>27.27</v>
       </c>
       <c r="O15">
-        <v>317.5</v>
+        <v>313.7</v>
       </c>
       <c r="P15">
-        <v>0.59</v>
+        <v>0.58</v>
       </c>
       <c r="Q15">
-        <v>0.59</v>
+        <v>0.62</v>
       </c>
       <c r="R15">
         <v>1.23</v>
       </c>
       <c r="S15">
-        <v>2.18</v>
+        <v>2.12</v>
       </c>
       <c r="T15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U15">
         <v>0</v>
@@ -1552,64 +1552,64 @@
         <v>38</v>
       </c>
       <c r="D16">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F16">
         <v>10</v>
       </c>
       <c r="G16">
-        <v>28.57</v>
+        <v>44.44</v>
       </c>
       <c r="H16">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I16">
-        <v>4090</v>
+        <v>5954</v>
       </c>
       <c r="J16">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="K16">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L16">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="M16">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="N16">
-        <v>21.05</v>
+        <v>30.19</v>
       </c>
       <c r="O16">
-        <v>292.1</v>
+        <v>330.8</v>
       </c>
       <c r="P16">
-        <v>0.57</v>
+        <v>0.89</v>
       </c>
       <c r="Q16">
-        <v>0.57</v>
+        <v>0.5</v>
       </c>
       <c r="R16">
-        <v>1</v>
+        <v>1.11</v>
       </c>
       <c r="S16">
-        <v>2.71</v>
+        <v>2.94</v>
       </c>
       <c r="T16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V16">
         <v>0</v>
       </c>
       <c r="W16">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="2:23">
@@ -1620,55 +1620,55 @@
         <v>38</v>
       </c>
       <c r="D17">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E17">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F17">
         <v>6</v>
       </c>
       <c r="G17">
-        <v>40</v>
+        <v>57.14</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17">
-        <v>3541</v>
+        <v>5291</v>
       </c>
       <c r="J17">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K17">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="L17">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="M17">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="N17">
-        <v>25</v>
+        <v>23.53</v>
       </c>
       <c r="O17">
-        <v>354.1</v>
+        <v>377.9</v>
       </c>
       <c r="P17">
-        <v>0.6</v>
+        <v>0.57</v>
       </c>
       <c r="Q17">
-        <v>0.9</v>
+        <v>0.86</v>
       </c>
       <c r="R17">
-        <v>1.3</v>
+        <v>1.86</v>
       </c>
       <c r="S17">
-        <v>2.4</v>
+        <v>2.43</v>
       </c>
       <c r="T17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U17">
         <v>0</v>
@@ -1677,7 +1677,7 @@
         <v>0</v>
       </c>
       <c r="W17">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="2:23">
@@ -1892,25 +1892,25 @@
         <v>43</v>
       </c>
       <c r="D21">
+        <v>18</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21">
         <v>16</v>
       </c>
-      <c r="E21">
-        <v>2</v>
-      </c>
-      <c r="F21">
-        <v>14</v>
-      </c>
       <c r="G21">
-        <v>12.5</v>
+        <v>11.11</v>
       </c>
       <c r="H21">
         <v>1</v>
       </c>
       <c r="I21">
-        <v>4037</v>
+        <v>4335</v>
       </c>
       <c r="J21">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K21">
         <v>6</v>
@@ -1919,25 +1919,25 @@
         <v>17</v>
       </c>
       <c r="M21">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="N21">
-        <v>46.67</v>
+        <v>40</v>
       </c>
       <c r="O21">
-        <v>252.3</v>
+        <v>240.8</v>
       </c>
       <c r="P21">
         <v>0.44</v>
       </c>
       <c r="Q21">
-        <v>0.38</v>
+        <v>0.33</v>
       </c>
       <c r="R21">
-        <v>1.06</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="S21">
-        <v>0.9399999999999999</v>
+        <v>1.11</v>
       </c>
       <c r="T21">
         <v>0</v>
@@ -1960,52 +1960,52 @@
         <v>43</v>
       </c>
       <c r="D22">
+        <v>31</v>
+      </c>
+      <c r="E22">
+        <v>8</v>
+      </c>
+      <c r="F22">
         <v>23</v>
       </c>
-      <c r="E22">
-        <v>6</v>
-      </c>
-      <c r="F22">
-        <v>17</v>
-      </c>
       <c r="G22">
-        <v>26.09</v>
+        <v>25.81</v>
       </c>
       <c r="H22">
         <v>2</v>
       </c>
       <c r="I22">
-        <v>7600</v>
+        <v>9650</v>
       </c>
       <c r="J22">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="K22">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="L22">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="M22">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="N22">
-        <v>29.41</v>
+        <v>29.03</v>
       </c>
       <c r="O22">
-        <v>330.4</v>
+        <v>311.3</v>
       </c>
       <c r="P22">
-        <v>0.65</v>
+        <v>0.58</v>
       </c>
       <c r="Q22">
-        <v>0.35</v>
+        <v>0.42</v>
       </c>
       <c r="R22">
-        <v>1.65</v>
+        <v>1.39</v>
       </c>
       <c r="S22">
-        <v>2.22</v>
+        <v>2</v>
       </c>
       <c r="T22">
         <v>2</v>
@@ -2028,52 +2028,52 @@
         <v>48</v>
       </c>
       <c r="D23">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E23">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F23">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G23">
-        <v>47.83</v>
+        <v>46.67</v>
       </c>
       <c r="H23">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I23">
-        <v>6984</v>
+        <v>8906</v>
       </c>
       <c r="J23">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="K23">
         <v>11</v>
       </c>
       <c r="L23">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="M23">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="N23">
-        <v>36.73</v>
+        <v>39.34</v>
       </c>
       <c r="O23">
-        <v>303.7</v>
+        <v>296.9</v>
       </c>
       <c r="P23">
-        <v>0.78</v>
+        <v>0.8</v>
       </c>
       <c r="Q23">
-        <v>0.48</v>
+        <v>0.37</v>
       </c>
       <c r="R23">
-        <v>1.17</v>
+        <v>1.07</v>
       </c>
       <c r="S23">
-        <v>2.13</v>
+        <v>2.03</v>
       </c>
       <c r="T23">
         <v>3</v>
@@ -2096,52 +2096,52 @@
         <v>48</v>
       </c>
       <c r="D24">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F24">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G24">
-        <v>42.11</v>
+        <v>40.91</v>
       </c>
       <c r="H24">
         <v>5</v>
       </c>
       <c r="I24">
-        <v>5971</v>
+        <v>6822</v>
       </c>
       <c r="J24">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="K24">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="L24">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="M24">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="N24">
-        <v>34.78</v>
+        <v>33.33</v>
       </c>
       <c r="O24">
-        <v>314.3</v>
+        <v>310.1</v>
       </c>
       <c r="P24">
-        <v>0.84</v>
+        <v>0.82</v>
       </c>
       <c r="Q24">
-        <v>0.37</v>
+        <v>0.45</v>
       </c>
       <c r="R24">
-        <v>1.11</v>
+        <v>1.05</v>
       </c>
       <c r="S24">
-        <v>2.42</v>
+        <v>2.45</v>
       </c>
       <c r="T24">
         <v>4</v>
@@ -2164,52 +2164,52 @@
         <v>48</v>
       </c>
       <c r="D25">
+        <v>19</v>
+      </c>
+      <c r="E25">
+        <v>12</v>
+      </c>
+      <c r="F25">
+        <v>7</v>
+      </c>
+      <c r="G25">
+        <v>63.16</v>
+      </c>
+      <c r="H25">
+        <v>4</v>
+      </c>
+      <c r="I25">
+        <v>5977</v>
+      </c>
+      <c r="J25">
+        <v>17</v>
+      </c>
+      <c r="K25">
+        <v>10</v>
+      </c>
+      <c r="L25">
         <v>13</v>
       </c>
-      <c r="E25">
-        <v>8</v>
-      </c>
-      <c r="F25">
-        <v>5</v>
-      </c>
-      <c r="G25">
-        <v>61.54</v>
-      </c>
-      <c r="H25">
+      <c r="M25">
+        <v>57</v>
+      </c>
+      <c r="N25">
+        <v>29.82</v>
+      </c>
+      <c r="O25">
+        <v>314.6</v>
+      </c>
+      <c r="P25">
+        <v>0.89</v>
+      </c>
+      <c r="Q25">
+        <v>0.53</v>
+      </c>
+      <c r="R25">
+        <v>0.68</v>
+      </c>
+      <c r="S25">
         <v>3</v>
-      </c>
-      <c r="I25">
-        <v>4202</v>
-      </c>
-      <c r="J25">
-        <v>13</v>
-      </c>
-      <c r="K25">
-        <v>6</v>
-      </c>
-      <c r="L25">
-        <v>8</v>
-      </c>
-      <c r="M25">
-        <v>43</v>
-      </c>
-      <c r="N25">
-        <v>30.23</v>
-      </c>
-      <c r="O25">
-        <v>323.2</v>
-      </c>
-      <c r="P25">
-        <v>1</v>
-      </c>
-      <c r="Q25">
-        <v>0.46</v>
-      </c>
-      <c r="R25">
-        <v>0.62</v>
-      </c>
-      <c r="S25">
-        <v>3.31</v>
       </c>
       <c r="T25">
         <v>2</v>
@@ -2232,64 +2232,64 @@
         <v>48</v>
       </c>
       <c r="D26">
+        <v>23</v>
+      </c>
+      <c r="E26">
+        <v>9</v>
+      </c>
+      <c r="F26">
+        <v>14</v>
+      </c>
+      <c r="G26">
+        <v>39.13</v>
+      </c>
+      <c r="H26">
+        <v>2</v>
+      </c>
+      <c r="I26">
+        <v>6515</v>
+      </c>
+      <c r="J26">
         <v>15</v>
       </c>
-      <c r="E26">
-        <v>5</v>
-      </c>
-      <c r="F26">
-        <v>10</v>
-      </c>
-      <c r="G26">
-        <v>33.33</v>
-      </c>
-      <c r="H26">
-        <v>0</v>
-      </c>
-      <c r="I26">
-        <v>3544</v>
-      </c>
-      <c r="J26">
-        <v>7</v>
-      </c>
       <c r="K26">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="L26">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="M26">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="N26">
-        <v>25.93</v>
+        <v>28.85</v>
       </c>
       <c r="O26">
-        <v>236.3</v>
+        <v>283.3</v>
       </c>
       <c r="P26">
-        <v>0.47</v>
+        <v>0.65</v>
       </c>
       <c r="Q26">
-        <v>0.33</v>
+        <v>0.57</v>
       </c>
       <c r="R26">
-        <v>0.73</v>
+        <v>1.04</v>
       </c>
       <c r="S26">
-        <v>1.8</v>
+        <v>2.26</v>
       </c>
       <c r="T26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V26">
         <v>0</v>
       </c>
       <c r="W26">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="2:23">
@@ -2300,55 +2300,55 @@
         <v>53</v>
       </c>
       <c r="D27">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E27">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F27">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G27">
-        <v>45.45</v>
+        <v>48.15</v>
       </c>
       <c r="H27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I27">
-        <v>5603</v>
+        <v>7266</v>
       </c>
       <c r="J27">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="K27">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L27">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="M27">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="N27">
-        <v>39.29</v>
+        <v>40</v>
       </c>
       <c r="O27">
-        <v>254.7</v>
+        <v>269.1</v>
       </c>
       <c r="P27">
-        <v>0.5</v>
+        <v>0.52</v>
       </c>
       <c r="Q27">
-        <v>0.32</v>
+        <v>0.3</v>
       </c>
       <c r="R27">
-        <v>1.05</v>
+        <v>1.15</v>
       </c>
       <c r="S27">
-        <v>1.27</v>
+        <v>1.3</v>
       </c>
       <c r="T27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U27">
         <v>0</v>
@@ -2357,7 +2357,7 @@
         <v>0</v>
       </c>
       <c r="W27">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="2:23">
@@ -2368,55 +2368,55 @@
         <v>53</v>
       </c>
       <c r="D28">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E28">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F28">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G28">
-        <v>47.37</v>
+        <v>50</v>
       </c>
       <c r="H28">
         <v>3</v>
       </c>
       <c r="I28">
-        <v>4841</v>
+        <v>6443</v>
       </c>
       <c r="J28">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K28">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="L28">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="M28">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="N28">
-        <v>26.09</v>
+        <v>21.88</v>
       </c>
       <c r="O28">
-        <v>254.8</v>
+        <v>268.5</v>
       </c>
       <c r="P28">
-        <v>0.32</v>
+        <v>0.29</v>
       </c>
       <c r="Q28">
-        <v>0.37</v>
+        <v>0.42</v>
       </c>
       <c r="R28">
-        <v>1.11</v>
+        <v>1.08</v>
       </c>
       <c r="S28">
-        <v>1.21</v>
+        <v>1.33</v>
       </c>
       <c r="T28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U28">
         <v>0</v>
@@ -2425,7 +2425,7 @@
         <v>0</v>
       </c>
       <c r="W28">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="2:23">
@@ -2436,55 +2436,55 @@
         <v>53</v>
       </c>
       <c r="D29">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E29">
+        <v>13</v>
+      </c>
+      <c r="F29">
+        <v>13</v>
+      </c>
+      <c r="G29">
+        <v>50</v>
+      </c>
+      <c r="H29">
+        <v>8</v>
+      </c>
+      <c r="I29">
+        <v>10186</v>
+      </c>
+      <c r="J29">
+        <v>26</v>
+      </c>
+      <c r="K29">
         <v>10</v>
       </c>
-      <c r="F29">
-        <v>11</v>
-      </c>
-      <c r="G29">
-        <v>47.62</v>
-      </c>
-      <c r="H29">
-        <v>6</v>
-      </c>
-      <c r="I29">
-        <v>7819</v>
-      </c>
-      <c r="J29">
-        <v>20</v>
-      </c>
-      <c r="K29">
-        <v>7</v>
-      </c>
       <c r="L29">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="M29">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="N29">
-        <v>35.09</v>
+        <v>32.91</v>
       </c>
       <c r="O29">
-        <v>372.3</v>
+        <v>391.8</v>
       </c>
       <c r="P29">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="Q29">
-        <v>0.33</v>
+        <v>0.38</v>
       </c>
       <c r="R29">
-        <v>1.48</v>
+        <v>1.54</v>
       </c>
       <c r="S29">
-        <v>2.71</v>
+        <v>3.04</v>
       </c>
       <c r="T29">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="U29">
         <v>1</v>
@@ -2493,7 +2493,7 @@
         <v>0</v>
       </c>
       <c r="W29">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="2:23">
@@ -2572,52 +2572,52 @@
         <v>58</v>
       </c>
       <c r="D31">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E31">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F31">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G31">
-        <v>76.19</v>
+        <v>76</v>
       </c>
       <c r="H31">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I31">
-        <v>9260</v>
+        <v>10794</v>
       </c>
       <c r="J31">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="K31">
         <v>16</v>
       </c>
       <c r="L31">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="M31">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="N31">
-        <v>56.45</v>
+        <v>54.79</v>
       </c>
       <c r="O31">
-        <v>441</v>
+        <v>431.8</v>
       </c>
       <c r="P31">
-        <v>1.67</v>
+        <v>1.6</v>
       </c>
       <c r="Q31">
-        <v>0.76</v>
+        <v>0.64</v>
       </c>
       <c r="R31">
-        <v>0.76</v>
+        <v>0.92</v>
       </c>
       <c r="S31">
-        <v>2.95</v>
+        <v>2.92</v>
       </c>
       <c r="T31">
         <v>6</v>
@@ -2629,7 +2629,7 @@
         <v>2</v>
       </c>
       <c r="W31">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="2:23">
@@ -2640,52 +2640,52 @@
         <v>58</v>
       </c>
       <c r="D32">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E32">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F32">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G32">
         <v>66.67</v>
       </c>
       <c r="H32">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I32">
-        <v>6711</v>
+        <v>7441</v>
       </c>
       <c r="J32">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K32">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="L32">
         <v>15</v>
       </c>
       <c r="M32">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="N32">
-        <v>55.32</v>
+        <v>55.1</v>
       </c>
       <c r="O32">
-        <v>372.8</v>
+        <v>354.3</v>
       </c>
       <c r="P32">
-        <v>1.44</v>
+        <v>1.29</v>
       </c>
       <c r="Q32">
-        <v>0.72</v>
+        <v>0.76</v>
       </c>
       <c r="R32">
-        <v>0.83</v>
+        <v>0.71</v>
       </c>
       <c r="S32">
-        <v>2.61</v>
+        <v>2.33</v>
       </c>
       <c r="T32">
         <v>3</v>
@@ -2708,52 +2708,52 @@
         <v>58</v>
       </c>
       <c r="D33">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E33">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F33">
         <v>6</v>
       </c>
       <c r="G33">
-        <v>64.70999999999999</v>
+        <v>68.42</v>
       </c>
       <c r="H33">
         <v>3</v>
       </c>
       <c r="I33">
-        <v>5207</v>
+        <v>5765</v>
       </c>
       <c r="J33">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K33">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="L33">
         <v>9</v>
       </c>
       <c r="M33">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="N33">
-        <v>42.42</v>
+        <v>41.03</v>
       </c>
       <c r="O33">
-        <v>306.3</v>
+        <v>303.4</v>
       </c>
       <c r="P33">
-        <v>0.82</v>
+        <v>0.84</v>
       </c>
       <c r="Q33">
         <v>1</v>
       </c>
       <c r="R33">
-        <v>0.53</v>
+        <v>0.47</v>
       </c>
       <c r="S33">
-        <v>1.94</v>
+        <v>2.05</v>
       </c>
       <c r="T33">
         <v>2</v>
@@ -2776,55 +2776,55 @@
         <v>58</v>
       </c>
       <c r="D34">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E34">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F34">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G34">
-        <v>69.23</v>
+        <v>68.75</v>
       </c>
       <c r="H34">
         <v>0</v>
       </c>
       <c r="I34">
-        <v>3801</v>
+        <v>4538</v>
       </c>
       <c r="J34">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K34">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="L34">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M34">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="N34">
-        <v>65.22</v>
+        <v>59.26</v>
       </c>
       <c r="O34">
-        <v>292.4</v>
+        <v>283.6</v>
       </c>
       <c r="P34">
-        <v>1.15</v>
+        <v>1</v>
       </c>
       <c r="Q34">
-        <v>0.77</v>
+        <v>0.75</v>
       </c>
       <c r="R34">
-        <v>0.46</v>
+        <v>0.5</v>
       </c>
       <c r="S34">
-        <v>1.77</v>
+        <v>1.69</v>
       </c>
       <c r="T34">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U34">
         <v>2</v>

</xml_diff>